<commit_message>
changed microsoft.office.interop.excel to NOPI
</commit_message>
<xml_diff>
--- a/Assets/CommandConditions.xlsx
+++ b/Assets/CommandConditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\visualstudio workstation\TheMoneyIsAlwaysRight\TheMoneyIsAlwaysRight\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BA2E28-39CA-40AC-B422-24F132ADEA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F810A48-277F-4DEB-8EDA-200A19CA0ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CA94E46-E504-4B77-99CE-16158E15C93D}"/>
+    <workbookView xWindow="5745" yWindow="1260" windowWidth="21600" windowHeight="11385" xr2:uid="{6CA94E46-E504-4B77-99CE-16158E15C93D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>ExitGame</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#EOF</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -423,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D22047AE-371C-4F7F-9031-D5FE88443970}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -451,6 +455,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>